<commit_message>
Corrected normalization & added nore prelim stats
</commit_message>
<xml_diff>
--- a/KEGG/ko_comp.xlsx
+++ b/KEGG/ko_comp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chian\Documents\GitHub\Squirrel_MetaG\KEGG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60BD51FA-4F3A-4E6C-9B62-101527D425E2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920D2D92-8554-47FE-A21A-72A68545F5CC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="9792" windowHeight="5820" xr2:uid="{CD56A5D8-1979-42CD-8554-E1A96962EF37}"/>
   </bookViews>
@@ -538,12 +538,12 @@
   <dimension ref="A1:AB19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB20" sqref="AB20"/>
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="19.21875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -706,8 +706,8 @@
         <v>17014</v>
       </c>
       <c r="Z2">
-        <f>SUM(C2:Y2)</f>
-        <v>145126</v>
+        <f>C2+P2+U2+Y2</f>
+        <v>81070</v>
       </c>
       <c r="AA2" t="s">
         <v>45</v>
@@ -793,8 +793,8 @@
         <v>9453</v>
       </c>
       <c r="Z3">
-        <f t="shared" ref="Z3:Z19" si="0">SUM(C3:Y3)</f>
-        <v>92453</v>
+        <f t="shared" ref="Z3:Z19" si="0">C3+P3+U3+Y3</f>
+        <v>50953</v>
       </c>
       <c r="AA3" t="s">
         <v>46</v>
@@ -881,7 +881,7 @@
       </c>
       <c r="Z4">
         <f t="shared" si="0"/>
-        <v>229006</v>
+        <v>125622</v>
       </c>
       <c r="AA4" t="s">
         <v>45</v>
@@ -968,7 +968,7 @@
       </c>
       <c r="Z5">
         <f t="shared" si="0"/>
-        <v>168209</v>
+        <v>91649</v>
       </c>
       <c r="AA5" t="s">
         <v>46</v>
@@ -1055,7 +1055,7 @@
       </c>
       <c r="Z6">
         <f t="shared" si="0"/>
-        <v>188931</v>
+        <v>102202</v>
       </c>
       <c r="AA6" t="s">
         <v>45</v>
@@ -1142,7 +1142,7 @@
       </c>
       <c r="Z7">
         <f t="shared" si="0"/>
-        <v>118579</v>
+        <v>64054</v>
       </c>
       <c r="AA7" t="s">
         <v>46</v>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="Z8">
         <f t="shared" si="0"/>
-        <v>205322</v>
+        <v>110729</v>
       </c>
       <c r="AA8" t="s">
         <v>45</v>
@@ -1316,7 +1316,7 @@
       </c>
       <c r="Z9">
         <f t="shared" si="0"/>
-        <v>126431</v>
+        <v>68124</v>
       </c>
       <c r="AA9" t="s">
         <v>46</v>
@@ -1403,7 +1403,7 @@
       </c>
       <c r="Z10">
         <f t="shared" si="0"/>
-        <v>321708</v>
+        <v>175311</v>
       </c>
       <c r="AA10" t="s">
         <v>45</v>
@@ -1490,7 +1490,7 @@
       </c>
       <c r="Z11">
         <f t="shared" si="0"/>
-        <v>176529</v>
+        <v>95931</v>
       </c>
       <c r="AA11" t="s">
         <v>46</v>
@@ -1577,7 +1577,7 @@
       </c>
       <c r="Z12">
         <f t="shared" si="0"/>
-        <v>252423</v>
+        <v>136648</v>
       </c>
       <c r="AA12" t="s">
         <v>45</v>
@@ -1664,7 +1664,7 @@
       </c>
       <c r="Z13">
         <f t="shared" si="0"/>
-        <v>161400</v>
+        <v>87159</v>
       </c>
       <c r="AA13" t="s">
         <v>46</v>
@@ -1751,7 +1751,7 @@
       </c>
       <c r="Z14">
         <f t="shared" si="0"/>
-        <v>151161</v>
+        <v>82219</v>
       </c>
       <c r="AA14" t="s">
         <v>45</v>
@@ -1838,7 +1838,7 @@
       </c>
       <c r="Z15">
         <f t="shared" si="0"/>
-        <v>100281</v>
+        <v>54257</v>
       </c>
       <c r="AA15" t="s">
         <v>46</v>
@@ -1925,7 +1925,7 @@
       </c>
       <c r="Z16">
         <f t="shared" si="0"/>
-        <v>257853</v>
+        <v>145896</v>
       </c>
       <c r="AA16" t="s">
         <v>45</v>
@@ -2012,7 +2012,7 @@
       </c>
       <c r="Z17">
         <f t="shared" si="0"/>
-        <v>150955</v>
+        <v>84527</v>
       </c>
       <c r="AA17" t="s">
         <v>46</v>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="Z18">
         <f t="shared" si="0"/>
-        <v>245606</v>
+        <v>132518</v>
       </c>
       <c r="AA18" t="s">
         <v>45</v>
@@ -2186,7 +2186,7 @@
       </c>
       <c r="Z19">
         <f t="shared" si="0"/>
-        <v>148115</v>
+        <v>79843</v>
       </c>
       <c r="AA19" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
Added kegg & dbcan barplots
</commit_message>
<xml_diff>
--- a/KEGG/ko_comp.xlsx
+++ b/KEGG/ko_comp.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chian\Documents\GitHub\Squirrel_MetaG\KEGG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920D2D92-8554-47FE-A21A-72A68545F5CC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D52B37-9F61-4CA2-BEAB-935D4F0D3024}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="9792" windowHeight="5820" xr2:uid="{CD56A5D8-1979-42CD-8554-E1A96962EF37}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="52">
   <si>
     <t>Metabolism</t>
   </si>
@@ -175,6 +175,12 @@
   </si>
   <si>
     <t>Spring</t>
+  </si>
+  <si>
+    <t>Other1</t>
+  </si>
+  <si>
+    <t>Total1</t>
   </si>
 </sst>
 </file>
@@ -535,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12099F47-71DD-4D2B-A19C-4C534DA15843}">
-  <dimension ref="A1:AB19"/>
+  <dimension ref="A1:AD19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
+      <selection activeCell="W28" sqref="W28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -546,7 +552,7 @@
     <col min="1" max="1" width="19.21875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>40</v>
       </c>
@@ -623,13 +629,19 @@
         <v>42</v>
       </c>
       <c r="AA1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -703,20 +715,28 @@
         <v>11</v>
       </c>
       <c r="Y2">
+        <f>SUM(F2+I2+J2+K2+L2+M2+N2+O2+Q2+R2+S2+T2+V2+W2+X2)</f>
+        <v>32696</v>
+      </c>
+      <c r="Z2">
+        <f>SUM(Y2+D2+E2+G2+H2)</f>
+        <v>64056</v>
+      </c>
+      <c r="AA2">
         <v>17014</v>
       </c>
-      <c r="Z2">
-        <f>C2+P2+U2+Y2</f>
+      <c r="AB2">
+        <f>C2+P2+U2+AA2</f>
         <v>81070</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AC2" t="s">
         <v>45</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AD2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -790,20 +810,28 @@
         <v>8</v>
       </c>
       <c r="Y3">
+        <f t="shared" ref="Y3:Y19" si="0">SUM(F3+I3+J3+K3+L3+M3+N3+O3+Q3+R3+S3+T3+V3+W3+X3)</f>
+        <v>21440</v>
+      </c>
+      <c r="Z3">
+        <f t="shared" ref="Z3:Z19" si="1">SUM(Y3+D3+E3+G3+H3)</f>
+        <v>41500</v>
+      </c>
+      <c r="AA3">
         <v>9453</v>
       </c>
-      <c r="Z3">
-        <f t="shared" ref="Z3:Z19" si="0">C3+P3+U3+Y3</f>
+      <c r="AB3">
+        <f>C3+P3+U3+AA3</f>
         <v>50953</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AC3" t="s">
         <v>46</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AD3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
@@ -877,20 +905,28 @@
         <v>26</v>
       </c>
       <c r="Y4">
+        <f t="shared" si="0"/>
+        <v>53051</v>
+      </c>
+      <c r="Z4">
+        <f t="shared" si="1"/>
+        <v>103384</v>
+      </c>
+      <c r="AA4">
         <v>22238</v>
       </c>
-      <c r="Z4">
-        <f t="shared" si="0"/>
+      <c r="AB4">
+        <f>C4+P4+U4+AA4</f>
         <v>125622</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AC4" t="s">
         <v>45</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AD4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -964,20 +1000,28 @@
         <v>19</v>
       </c>
       <c r="Y5">
+        <f t="shared" si="0"/>
+        <v>39805</v>
+      </c>
+      <c r="Z5">
+        <f t="shared" si="1"/>
+        <v>76560</v>
+      </c>
+      <c r="AA5">
         <v>15089</v>
       </c>
-      <c r="Z5">
-        <f t="shared" si="0"/>
+      <c r="AB5">
+        <f>C5+P5+U5+AA5</f>
         <v>91649</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AC5" t="s">
         <v>46</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AD5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
@@ -1051,20 +1095,28 @@
         <v>16</v>
       </c>
       <c r="Y6">
+        <f t="shared" si="0"/>
+        <v>43014</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" si="1"/>
+        <v>86729</v>
+      </c>
+      <c r="AA6">
         <v>15473</v>
       </c>
-      <c r="Z6">
-        <f t="shared" si="0"/>
+      <c r="AB6">
+        <f>C6+P6+U6+AA6</f>
         <v>102202</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AC6" t="s">
         <v>45</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AD6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -1138,20 +1190,28 @@
         <v>10</v>
       </c>
       <c r="Y7">
+        <f t="shared" si="0"/>
+        <v>27818</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" si="1"/>
+        <v>54525</v>
+      </c>
+      <c r="AA7">
         <v>9529</v>
       </c>
-      <c r="Z7">
-        <f t="shared" si="0"/>
+      <c r="AB7">
+        <f>C7+P7+U7+AA7</f>
         <v>64054</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AC7" t="s">
         <v>46</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AD7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
@@ -1225,20 +1285,28 @@
         <v>22</v>
       </c>
       <c r="Y8">
+        <f t="shared" si="0"/>
+        <v>47100</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" si="1"/>
+        <v>94593</v>
+      </c>
+      <c r="AA8">
         <v>16136</v>
       </c>
-      <c r="Z8">
-        <f t="shared" si="0"/>
+      <c r="AB8">
+        <f>C8+P8+U8+AA8</f>
         <v>110729</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AC8" t="s">
         <v>45</v>
       </c>
-      <c r="AB8" t="s">
+      <c r="AD8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
@@ -1312,20 +1380,28 @@
         <v>15</v>
       </c>
       <c r="Y9">
+        <f t="shared" si="0"/>
+        <v>30074</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" si="1"/>
+        <v>58307</v>
+      </c>
+      <c r="AA9">
         <v>9817</v>
       </c>
-      <c r="Z9">
-        <f t="shared" si="0"/>
+      <c r="AB9">
+        <f>C9+P9+U9+AA9</f>
         <v>68124</v>
       </c>
-      <c r="AA9" t="s">
+      <c r="AC9" t="s">
         <v>46</v>
       </c>
-      <c r="AB9" t="s">
+      <c r="AD9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -1399,20 +1475,28 @@
         <v>27</v>
       </c>
       <c r="Y10">
+        <f t="shared" si="0"/>
+        <v>72340</v>
+      </c>
+      <c r="Z10">
+        <f t="shared" si="1"/>
+        <v>146397</v>
+      </c>
+      <c r="AA10">
         <v>28914</v>
       </c>
-      <c r="Z10">
-        <f t="shared" si="0"/>
+      <c r="AB10">
+        <f>C10+P10+U10+AA10</f>
         <v>175311</v>
       </c>
-      <c r="AA10" t="s">
+      <c r="AC10" t="s">
         <v>45</v>
       </c>
-      <c r="AB10" t="s">
+      <c r="AD10" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
@@ -1486,20 +1570,28 @@
         <v>17</v>
       </c>
       <c r="Y11">
+        <f t="shared" si="0"/>
+        <v>41179</v>
+      </c>
+      <c r="Z11">
+        <f t="shared" si="1"/>
+        <v>80598</v>
+      </c>
+      <c r="AA11">
         <v>15333</v>
       </c>
-      <c r="Z11">
-        <f t="shared" si="0"/>
+      <c r="AB11">
+        <f>C11+P11+U11+AA11</f>
         <v>95931</v>
       </c>
-      <c r="AA11" t="s">
+      <c r="AC11" t="s">
         <v>46</v>
       </c>
-      <c r="AB11" t="s">
+      <c r="AD11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -1573,20 +1665,28 @@
         <v>17</v>
       </c>
       <c r="Y12">
+        <f t="shared" si="0"/>
+        <v>57643</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" si="1"/>
+        <v>115775</v>
+      </c>
+      <c r="AA12">
         <v>20873</v>
       </c>
-      <c r="Z12">
-        <f t="shared" si="0"/>
+      <c r="AB12">
+        <f>C12+P12+U12+AA12</f>
         <v>136648</v>
       </c>
-      <c r="AA12" t="s">
+      <c r="AC12" t="s">
         <v>45</v>
       </c>
-      <c r="AB12" t="s">
+      <c r="AD12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
@@ -1660,20 +1760,28 @@
         <v>16</v>
       </c>
       <c r="Y13">
+        <f t="shared" si="0"/>
+        <v>38045</v>
+      </c>
+      <c r="Z13">
+        <f t="shared" si="1"/>
+        <v>74241</v>
+      </c>
+      <c r="AA13">
         <v>12918</v>
       </c>
-      <c r="Z13">
-        <f t="shared" si="0"/>
+      <c r="AB13">
+        <f>C13+P13+U13+AA13</f>
         <v>87159</v>
       </c>
-      <c r="AA13" t="s">
+      <c r="AC13" t="s">
         <v>46</v>
       </c>
-      <c r="AB13" t="s">
+      <c r="AD13" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>34</v>
       </c>
@@ -1747,20 +1855,28 @@
         <v>19</v>
       </c>
       <c r="Y14">
+        <f t="shared" si="0"/>
+        <v>35551</v>
+      </c>
+      <c r="Z14">
+        <f t="shared" si="1"/>
+        <v>68942</v>
+      </c>
+      <c r="AA14">
         <v>13277</v>
       </c>
-      <c r="Z14">
-        <f t="shared" si="0"/>
+      <c r="AB14">
+        <f>C14+P14+U14+AA14</f>
         <v>82219</v>
       </c>
-      <c r="AA14" t="s">
+      <c r="AC14" t="s">
         <v>45</v>
       </c>
-      <c r="AB14" t="s">
+      <c r="AD14" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>35</v>
       </c>
@@ -1834,20 +1950,28 @@
         <v>13</v>
       </c>
       <c r="Y15">
+        <f t="shared" si="0"/>
+        <v>24060</v>
+      </c>
+      <c r="Z15">
+        <f t="shared" si="1"/>
+        <v>46024</v>
+      </c>
+      <c r="AA15">
         <v>8233</v>
       </c>
-      <c r="Z15">
-        <f t="shared" si="0"/>
+      <c r="AB15">
+        <f>C15+P15+U15+AA15</f>
         <v>54257</v>
       </c>
-      <c r="AA15" t="s">
+      <c r="AC15" t="s">
         <v>46</v>
       </c>
-      <c r="AB15" t="s">
+      <c r="AD15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>36</v>
       </c>
@@ -1921,20 +2045,28 @@
         <v>21</v>
       </c>
       <c r="Y16">
+        <f t="shared" si="0"/>
+        <v>57914</v>
+      </c>
+      <c r="Z16">
+        <f t="shared" si="1"/>
+        <v>111957</v>
+      </c>
+      <c r="AA16">
         <v>33939</v>
       </c>
-      <c r="Z16">
-        <f t="shared" si="0"/>
+      <c r="AB16">
+        <f>C16+P16+U16+AA16</f>
         <v>145896</v>
       </c>
-      <c r="AA16" t="s">
+      <c r="AC16" t="s">
         <v>45</v>
       </c>
-      <c r="AB16" t="s">
+      <c r="AD16" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>37</v>
       </c>
@@ -2008,20 +2140,28 @@
         <v>12</v>
       </c>
       <c r="Y17">
+        <f t="shared" si="0"/>
+        <v>35208</v>
+      </c>
+      <c r="Z17">
+        <f t="shared" si="1"/>
+        <v>66428</v>
+      </c>
+      <c r="AA17">
         <v>18099</v>
       </c>
-      <c r="Z17">
-        <f t="shared" si="0"/>
+      <c r="AB17">
+        <f>C17+P17+U17+AA17</f>
         <v>84527</v>
       </c>
-      <c r="AA17" t="s">
+      <c r="AC17" t="s">
         <v>46</v>
       </c>
-      <c r="AB17" t="s">
+      <c r="AD17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>38</v>
       </c>
@@ -2095,20 +2235,28 @@
         <v>17</v>
       </c>
       <c r="Y18">
+        <f t="shared" si="0"/>
+        <v>55326</v>
+      </c>
+      <c r="Z18">
+        <f t="shared" si="1"/>
+        <v>113088</v>
+      </c>
+      <c r="AA18">
         <v>19430</v>
       </c>
-      <c r="Z18">
-        <f t="shared" si="0"/>
+      <c r="AB18">
+        <f>C18+P18+U18+AA18</f>
         <v>132518</v>
       </c>
-      <c r="AA18" t="s">
+      <c r="AC18" t="s">
         <v>45</v>
       </c>
-      <c r="AB18" t="s">
+      <c r="AD18" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>39</v>
       </c>
@@ -2182,16 +2330,24 @@
         <v>13</v>
       </c>
       <c r="Y19">
+        <f t="shared" si="0"/>
+        <v>34400</v>
+      </c>
+      <c r="Z19">
+        <f t="shared" si="1"/>
+        <v>68272</v>
+      </c>
+      <c r="AA19">
         <v>11571</v>
       </c>
-      <c r="Z19">
-        <f t="shared" si="0"/>
+      <c r="AB19">
+        <f>C19+P19+U19+AA19</f>
         <v>79843</v>
       </c>
-      <c r="AA19" t="s">
+      <c r="AC19" t="s">
         <v>46</v>
       </c>
-      <c r="AB19" t="s">
+      <c r="AD19" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>